<commit_message>
AG: se continúa con la elaboración de los diccionarios
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_06.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_06.xlsx
@@ -5,17 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angleito\Documents\Consultorías\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="04_1_general" sheetId="11" r:id="rId1"/>
-    <sheet name="04_1_diccionario" sheetId="10" r:id="rId2"/>
+    <sheet name="06_1_general" sheetId="11" r:id="rId1"/>
+    <sheet name="06_1_diccionario" sheetId="10" r:id="rId2"/>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId3"/>
+    <sheet name="06_2_general" sheetId="12" r:id="rId4"/>
+    <sheet name="06_2_diccionario" sheetId="13" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="186">
   <si>
     <t>Elemento</t>
   </si>
@@ -311,13 +316,290 @@
   </si>
   <si>
     <t>Medios de Conservación y Manejo Ex Situ</t>
+  </si>
+  <si>
+    <t>Identificación</t>
+  </si>
+  <si>
+    <t>Transacción o Evento</t>
+  </si>
+  <si>
+    <t>Retencion</t>
+  </si>
+  <si>
+    <t>A7:AL57</t>
+  </si>
+  <si>
+    <t>Causal COIP / CODA</t>
+  </si>
+  <si>
+    <t>Fecha de la retención</t>
+  </si>
+  <si>
+    <t>Hora de la retención</t>
+  </si>
+  <si>
+    <t>Dirección para notificaciones</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
+    <t>Lugar</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Costo monetario</t>
+  </si>
+  <si>
+    <t>Peso/Volumen</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Acta Destino Final</t>
+  </si>
+  <si>
+    <t>Tipo de proceso</t>
+  </si>
+  <si>
+    <t>Razón social</t>
+  </si>
+  <si>
+    <t>Código del acta de la retención</t>
+  </si>
+  <si>
+    <t>Causal de la retenciónsegún el COIP o CODA</t>
+  </si>
+  <si>
+    <t>Fecha en la que se realizó la retención</t>
+  </si>
+  <si>
+    <t>Hora en la que se realizaó la retención</t>
+  </si>
+  <si>
+    <t>Coordenadas UTM Longitud</t>
+  </si>
+  <si>
+    <t>Coordenada UTM Longitud</t>
+  </si>
+  <si>
+    <t>Coordenada UTM Latidud</t>
+  </si>
+  <si>
+    <t>Coordenadas UTM Latitud</t>
+  </si>
+  <si>
+    <t>Nombres del Infractor</t>
+  </si>
+  <si>
+    <t>Apellidos del Infractor</t>
+  </si>
+  <si>
+    <t>Cédula o pasaporte del infractor</t>
+  </si>
+  <si>
+    <t>Dirección del infractor para realizar notificaciones</t>
+  </si>
+  <si>
+    <t>Tipo de transporte en el que se llevaba la vida silvestre</t>
+  </si>
+  <si>
+    <t>Placa del transporte en el que se llevaba la vida silvestre</t>
+  </si>
+  <si>
+    <t>Clase de transporte en el que se llevaba la vida silvestre</t>
+  </si>
+  <si>
+    <t>Lugar donde se tenía el escondite de la vida silvestre</t>
+  </si>
+  <si>
+    <t>Detalle del escondite</t>
+  </si>
+  <si>
+    <t>Reino al que pertenece la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Clase a la que pertenece la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Nombre científico de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Nombre común de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Forma o estado de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Cantidad de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Costo monetario de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Etapa de vida de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Número de machos de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Númer de hembras de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Número de sexo indeterminado de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Estado físico de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Detalle del elemento constituvio de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Peso o volumen de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Unidad de medida del peso o volumen de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Destino final de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Acta del destino final de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Tipo de proceso con respecto al proceso de la retención de la vida silvestre</t>
+  </si>
+  <si>
+    <t>Número de proceso respecto al proceso de la retención de la vida silvestre</t>
+  </si>
+  <si>
+    <t>Nombres del lugar de destino dela vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Nombres del responsable de larecepción de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Apellidos del responsable de la recepción de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Fecha de recepción de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Registro de la infracción o delito</t>
+  </si>
+  <si>
+    <t>Datos del infractor</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Datos de la vida silvestre retenida</t>
+  </si>
+  <si>
+    <t>Información Administrativa MAE</t>
+  </si>
+  <si>
+    <t>No. de proceso</t>
+  </si>
+  <si>
+    <t>Tenencia ilegal</t>
+  </si>
+  <si>
+    <t>Luis Eugenio</t>
+  </si>
+  <si>
+    <t>Duarte Acevedo</t>
+  </si>
+  <si>
+    <t>1500229073</t>
+  </si>
+  <si>
+    <t>Barrio Central, El Coca</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Mammalia - 45471</t>
+  </si>
+  <si>
+    <t>Cuniculus paca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guanta </t>
+  </si>
+  <si>
+    <t>Elementos constitutivos</t>
+  </si>
+  <si>
+    <t>Carne</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Entierro</t>
+  </si>
+  <si>
+    <t>01-2020-EN-DPAO</t>
+  </si>
+  <si>
+    <t>Penal</t>
+  </si>
+  <si>
+    <t>Privado</t>
+  </si>
+  <si>
+    <t>Fluvial</t>
+  </si>
+  <si>
+    <t>Otro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los elementos constitutivos estaban en una olla </t>
+  </si>
+  <si>
+    <t>SBD0008</t>
+  </si>
+  <si>
+    <t>Adulto</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>06-PNT-2020</t>
+  </si>
+  <si>
+    <t>Hospital de fauna silvestre Tueri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis </t>
+  </si>
+  <si>
+    <t>Rosero</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,6 +614,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -378,10 +679,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -408,8 +710,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -423,6 +734,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Rescate"/>
+      <sheetName val="Retencion"/>
+      <sheetName val="Catalogos"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,7 +1019,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,6 +1174,9 @@
       <c r="F2" s="11" t="s">
         <v>90</v>
       </c>
+      <c r="H2" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -867,6 +1198,9 @@
       <c r="F3" s="11" t="s">
         <v>90</v>
       </c>
+      <c r="H3" s="11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -893,7 +1227,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>89</v>
@@ -913,7 +1247,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>89</v>
@@ -1383,4 +1717,1168 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I3" s="15">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.4375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="I5" s="11">
+        <v>947257380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="11">
+        <v>9947538900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I22" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I27" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I30" s="11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="I39" s="15">
+        <v>43991</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>